<commit_message>
Before merging Assignment 3 final (Derek)
</commit_message>
<xml_diff>
--- a/FIT3158 - Case 1 - Assignment -Jing.xlsx
+++ b/FIT3158 - Case 1 - Assignment -Jing.xlsx
@@ -1,86 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jing\Dropbox\Monash Uni\FIT3158\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjsa3\Documents\GitHub\FIT3158---Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA8C118-9F9B-4B13-838D-4AB983CE2A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA415195-2CB6-487D-954C-3CEDB7AB6A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Freigh Loading Plan (LP model)" sheetId="1" r:id="rId1"/>
-    <sheet name="Sensitivity Report" sheetId="2" r:id="rId2"/>
-    <sheet name="Answer Report" sheetId="3" r:id="rId3"/>
+    <sheet name="Cover_page" sheetId="4" r:id="rId1"/>
+    <sheet name="Freigh Loading Plan (LP model)" sheetId="1" r:id="rId2"/>
+    <sheet name="Sensitivity Report" sheetId="2" r:id="rId3"/>
+    <sheet name="Answer Report" sheetId="3" r:id="rId4"/>
+    <sheet name="Report" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$9:$E$12</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$13</definedName>
-    <definedName name="solver_lhs10" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$H$9:$H$12</definedName>
-    <definedName name="solver_lhs11" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$H$9:$H$12</definedName>
-    <definedName name="solver_lhs12" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$H$9:$H$12</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$13</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$13:$E$13</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$14:$E$14</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$24</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$24</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$F$9:$F$12</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$F$9:$F$12</definedName>
-    <definedName name="solver_lhs9" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$H$9:$H$12</definedName>
-    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">7</definedName>
-    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$H$18</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel11" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel12" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$19</definedName>
-    <definedName name="solver_rhs10" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$I$9:$I$12</definedName>
-    <definedName name="solver_rhs11" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$I$9:$I$12</definedName>
-    <definedName name="solver_rhs12" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$I$9:$I$12</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$20</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$16:$E$16</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$15:$E$15</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$23</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$B$22</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$G$9:$G$12</definedName>
-    <definedName name="solver_rhs8" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$G$9:$G$12</definedName>
-    <definedName name="solver_rhs9" localSheetId="0" hidden="1">'Freigh Loading Plan (LP model)'!$I$9:$I$12</definedName>
-    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$B$9:$E$12</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$B$17</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$H$9:$H$12</definedName>
+    <definedName name="solver_lhs11" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$H$9:$H$12</definedName>
+    <definedName name="solver_lhs12" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$H$9:$H$12</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$B$17</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$B$17:$E$17</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$B$19:$E$19</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$I$5</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$I$5</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$F$9:$F$12</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$F$9:$F$12</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$H$9:$H$12</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">7</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$B$21</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel11" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel12" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$F$3</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$I$9:$I$12</definedName>
+    <definedName name="solver_rhs11" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$I$9:$I$12</definedName>
+    <definedName name="solver_rhs12" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$I$9:$I$12</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$F$4</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$B$14:$E$14</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$B$13:$E$13</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$I$4</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$I$3</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$G$9:$G$12</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$G$9:$G$12</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">'Freigh Loading Plan (LP model)'!$I$9:$I$12</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -102,8 +104,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jason Siu</author>
+    <author>A satisfied Microsoft Office user</author>
+  </authors>
+  <commentList>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{A0B6ADED-C0FB-4B0B-A995-E3B05088DC80}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>B9:E12 are variable cells</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="1" shapeId="0" xr:uid="{96474978-1483-4021-8115-E745D526CE60}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Objective cell</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="148">
   <si>
     <t>Cargo Type</t>
   </si>
@@ -135,15 +174,9 @@
     <t>Placed (tons)</t>
   </si>
   <si>
-    <t>Shipped (tons)</t>
-  </si>
-  <si>
     <t>Capacity (tons)</t>
   </si>
   <si>
-    <t>Cargo hold constraint</t>
-  </si>
-  <si>
     <t>Available (tons)</t>
   </si>
   <si>
@@ -159,9 +192,6 @@
     <t>Shipped (cubic)</t>
   </si>
   <si>
-    <t>Tons</t>
-  </si>
-  <si>
     <t xml:space="preserve">Profit </t>
   </si>
   <si>
@@ -417,15 +447,6 @@
     <t>C4 Shipped (tons)</t>
   </si>
   <si>
-    <t>Total placed tons</t>
-  </si>
-  <si>
-    <t>Total placed cubic</t>
-  </si>
-  <si>
-    <t>Total center cargo holds</t>
-  </si>
-  <si>
     <t>Profit per ton ($)</t>
   </si>
   <si>
@@ -550,24 +571,34 @@
   </si>
   <si>
     <t>$F$12&lt;=$G$12</t>
+  </si>
+  <si>
+    <t>Total center cargo holds (tons)</t>
+  </si>
+  <si>
+    <t>Cargo hold constraint (tons)</t>
+  </si>
+  <si>
+    <t>Total placed (tons)</t>
+  </si>
+  <si>
+    <t>Total placed (cubic)</t>
+  </si>
+  <si>
+    <t>Shipped items (tons)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -586,19 +617,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="17"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -607,48 +665,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor indexed="47"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -770,102 +798,272 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,6 +1080,695 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4544449" cy="561949"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AC160E6-4A4D-BA83-52AC-578331E28F4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3365500" y="622300"/>
+          <a:ext cx="4544449" cy="561949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="3000"/>
+            <a:t>FIT3158 - Assignment</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="3000" baseline="0"/>
+            <a:t> Case I</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="3000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>269585</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>157404</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1820884" cy="374141"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0063DB-6338-93C5-F988-EA9060D0A7A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="269585" y="1262304"/>
+          <a:ext cx="1820884" cy="374141"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800" b="1"/>
+            <a:t>Case </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1"/>
+            <a:t>description:</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1800" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>467530</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85244</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8555820" cy="3521556"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56528C09-A03E-F5E6-51AA-9C7DB983B98F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="467530" y="1558444"/>
+          <a:ext cx="8555820" cy="3521556"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1500" b="1"/>
+            <a:t>Background </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>The </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Australia’s Antarctic Program </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> — </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>managed and delivered</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> by </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The Australian Antarctic Division (AAD) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>— is t</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>hree year-round research program. There are three</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> research stations — namely </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Casey, Davis, and Mawson</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> — </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> are maintained in Antarctica to run scientific and logistical operations together with a station at the sub-Antarctic Macquarie Island.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Each year the AAD charters ships and vessels for resupply and transport operations to these station bases.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Southern Lights Logistics (SLL) operates an ice strengthened cargo ship the “Noyina” for resupply operations and critical cargo delivery for the AAD. It has four</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> cargos and four loading plan. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1500" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Objectives</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Since</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> there is a limited budget for the funded program</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> throught this </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>mathematical modelling, we hope </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>to find the optimal way to ship these equipments. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1600" b="1" baseline="0"/>
+            <a:t>Navigation to the report</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>There are three sheets in this file:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- The first one is to </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>mathematically formulate the freight loading plan for the Noyina as an LP model;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>- the second one is a</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>ensitivity</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>report</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>- the third one is a</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>nswer report</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>- and</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> the third is a report we produce where to answer our managers about the scenario they concerns. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1146,523 +2033,495 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213A5E5A-2E1F-4E3D-AFB0-6243A3A9C1E2}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.7265625" style="9"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17">
-        <v>75</v>
-      </c>
-      <c r="C2" s="17">
-        <v>50</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="17">
-        <v>55</v>
-      </c>
-      <c r="C3" s="17">
-        <v>35</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="17">
-        <v>65</v>
-      </c>
-      <c r="C4" s="17">
-        <v>70</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="17">
-        <v>85</v>
-      </c>
-      <c r="C5" s="17">
-        <v>65</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="18">
-        <v>1744.2342342342067</v>
-      </c>
-      <c r="C9" s="17">
-        <v>873.33333333335838</v>
-      </c>
-      <c r="D9" s="17">
-        <v>350.00000000000057</v>
-      </c>
-      <c r="E9" s="19">
-        <v>1832.4324324324334</v>
-      </c>
-      <c r="F9" s="24">
-        <f>SUM(B9:E9)</f>
-        <v>4799.9999999999991</v>
-      </c>
-      <c r="G9" s="25">
-        <v>4800</v>
-      </c>
-      <c r="H9" s="26">
-        <f>SUM(B9:E9)*C2</f>
-        <v>239999.99999999994</v>
-      </c>
-      <c r="I9" s="26">
-        <f>G9*C2</f>
-        <v>240000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="18">
-        <v>0</v>
-      </c>
-      <c r="C10" s="17">
-        <v>0</v>
-      </c>
-      <c r="D10" s="17">
-        <v>2499.9999999999995</v>
-      </c>
-      <c r="E10" s="17">
-        <v>0</v>
-      </c>
-      <c r="F10" s="24">
-        <f t="shared" ref="F10:F12" si="0">SUM(B10:E10)</f>
-        <v>2499.9999999999995</v>
-      </c>
-      <c r="G10" s="25">
-        <v>2500</v>
-      </c>
-      <c r="H10" s="26">
-        <f>SUM(B10:E10)*C3</f>
-        <v>87499.999999999985</v>
-      </c>
-      <c r="I10" s="26">
-        <f>G10*C3</f>
-        <v>87500</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="18">
-        <v>0</v>
-      </c>
-      <c r="C11" s="17">
-        <v>0</v>
-      </c>
-      <c r="D11" s="17">
-        <v>0</v>
-      </c>
-      <c r="E11" s="17">
-        <v>1200</v>
-      </c>
-      <c r="F11" s="24">
-        <f t="shared" si="0"/>
-        <v>1200</v>
-      </c>
-      <c r="G11" s="25">
-        <v>1200</v>
-      </c>
-      <c r="H11" s="26">
-        <f>SUM(B11:E11)*C4</f>
-        <v>84000</v>
-      </c>
-      <c r="I11" s="26">
-        <f>G11*C4</f>
-        <v>84000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="20">
-        <v>833.33333333336054</v>
-      </c>
-      <c r="C12" s="21">
-        <v>866.66666666663912</v>
-      </c>
-      <c r="D12" s="21">
-        <v>0</v>
-      </c>
-      <c r="E12" s="21">
-        <v>0</v>
-      </c>
-      <c r="F12" s="24">
-        <f t="shared" si="0"/>
-        <v>1699.9999999999995</v>
-      </c>
-      <c r="G12" s="25">
-        <v>1700</v>
-      </c>
-      <c r="H12" s="26">
-        <f>SUM(B12:E12)*C5</f>
-        <v>110499.99999999997</v>
-      </c>
-      <c r="I12" s="26">
-        <f>G12*C5</f>
-        <v>110500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="22">
-        <f>SUM(B9:B12)</f>
-        <v>2577.5675675675675</v>
-      </c>
-      <c r="C13" s="22">
-        <f t="shared" ref="C13:E13" si="1">SUM(C9:C12)</f>
-        <v>1739.9999999999975</v>
-      </c>
-      <c r="D13" s="22">
-        <f t="shared" si="1"/>
-        <v>2850</v>
-      </c>
-      <c r="E13" s="22">
-        <f t="shared" si="1"/>
-        <v>3032.4324324324334</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="G13" s="28">
-        <f>SUM(B13:E13)</f>
-        <v>10199.999999999998</v>
-      </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="23">
-        <f>SUMPRODUCT(B9:B12,$C$2:$C$5)</f>
-        <v>141378.37837837875</v>
-      </c>
-      <c r="C14" s="23">
-        <f t="shared" ref="C14:E14" si="2">SUMPRODUCT(C9:C12,$C$2:$C$5)</f>
-        <v>99999.999999999462</v>
-      </c>
-      <c r="D14" s="23">
-        <f t="shared" si="2"/>
-        <v>105000.00000000001</v>
-      </c>
-      <c r="E14" s="23">
-        <f t="shared" si="2"/>
-        <v>175621.62162162166</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" s="28">
-        <f>SUM(B14:E14)</f>
-        <v>521999.99999999988</v>
-      </c>
-      <c r="H14" s="29"/>
-      <c r="I14" s="30"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="23">
-        <v>170000</v>
-      </c>
-      <c r="C15" s="23">
-        <v>100000</v>
-      </c>
-      <c r="D15" s="23">
-        <v>105000</v>
-      </c>
-      <c r="E15" s="23">
-        <v>180000</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="35">
-        <v>3000</v>
-      </c>
-      <c r="C16" s="35">
-        <v>3000</v>
-      </c>
-      <c r="D16" s="35">
-        <v>3000</v>
-      </c>
-      <c r="E16" s="35">
-        <v>4000</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="17">
-        <f>SUMPRODUCT(F9:F12,B2:B5)</f>
-        <v>719999.99999999988</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="14">
-        <f>E13*1.15</f>
-        <v>3487.297297297298</v>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="14">
-        <f>E13*0.85</f>
-        <v>2577.5675675675684</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="17">
-        <f>H18*0.9</f>
-        <v>647999.99999999988</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="16">
-        <f>G13*0.45</f>
-        <v>4589.9999999999991</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="16">
-        <f>G13*0.55</f>
-        <v>5609.9999999999991</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="16">
-        <f>SUM(C13:D13)</f>
-        <v>4589.9999999999973</v>
-      </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:I27"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.36328125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="31.08984375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="18" style="11" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.54296875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="19.6328125" style="11" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="H2" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10">
+        <v>75</v>
+      </c>
+      <c r="C3" s="10">
+        <v>50</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="10">
+        <f>E17*1.15</f>
+        <v>3487.297297297298</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="10">
+        <f>B18*0.45</f>
+        <v>53190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10">
+        <v>55</v>
+      </c>
+      <c r="C4" s="10">
+        <v>35</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10">
+        <f>E17*0.85</f>
+        <v>2577.5675675675684</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="10">
+        <f>B18*0.55</f>
+        <v>65010.000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10">
+        <v>65</v>
+      </c>
+      <c r="C5" s="10">
+        <v>70</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="10">
+        <f>SUM(C17:D17)</f>
+        <v>112590</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10">
+        <v>85</v>
+      </c>
+      <c r="C6" s="10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12"/>
+      <c r="B8" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="23">
+        <v>1744.2342342342067</v>
+      </c>
+      <c r="C9" s="23">
+        <v>873.33333333335838</v>
+      </c>
+      <c r="D9" s="23">
+        <v>350.00000000000057</v>
+      </c>
+      <c r="E9" s="23">
+        <v>1832.4324324324334</v>
+      </c>
+      <c r="F9" s="25">
+        <f>SUM(B9:E9)</f>
+        <v>4799.9999999999991</v>
+      </c>
+      <c r="G9" s="18">
+        <v>4800</v>
+      </c>
+      <c r="H9" s="10">
+        <f>SUM(B9:E9)*C3</f>
+        <v>239999.99999999994</v>
+      </c>
+      <c r="I9" s="10">
+        <f>G9*C3</f>
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="23">
+        <v>0</v>
+      </c>
+      <c r="C10" s="23">
+        <v>0</v>
+      </c>
+      <c r="D10" s="23">
+        <v>2499.9999999999995</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0</v>
+      </c>
+      <c r="F10" s="25">
+        <f t="shared" ref="F10:F12" si="0">SUM(B10:E10)</f>
+        <v>2499.9999999999995</v>
+      </c>
+      <c r="G10" s="21">
+        <v>2500</v>
+      </c>
+      <c r="H10" s="10">
+        <f>SUM(B10:E10)*C4</f>
+        <v>87499.999999999985</v>
+      </c>
+      <c r="I10" s="10">
+        <f>G10*C4</f>
+        <v>87500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="23">
+        <v>0</v>
+      </c>
+      <c r="C11" s="23">
+        <v>0</v>
+      </c>
+      <c r="D11" s="23">
+        <v>0</v>
+      </c>
+      <c r="E11" s="26">
+        <v>1200</v>
+      </c>
+      <c r="F11" s="25">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="G11" s="18">
+        <v>1200</v>
+      </c>
+      <c r="H11" s="10">
+        <f>SUM(B11:E11)*C5</f>
+        <v>84000</v>
+      </c>
+      <c r="I11" s="10">
+        <f>G11*C5</f>
+        <v>84000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="24">
+        <v>833.33333333336054</v>
+      </c>
+      <c r="C12" s="24">
+        <v>866.66666666663912</v>
+      </c>
+      <c r="D12" s="24">
+        <v>0</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0</v>
+      </c>
+      <c r="F12" s="25">
+        <f t="shared" si="0"/>
+        <v>1699.9999999999995</v>
+      </c>
+      <c r="G12" s="18">
+        <v>1700</v>
+      </c>
+      <c r="H12" s="10">
+        <f>SUM(B12:E12)*C6</f>
+        <v>110499.99999999997</v>
+      </c>
+      <c r="I12" s="10">
+        <f>G12*C6</f>
+        <v>110500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="20">
+        <v>170000</v>
+      </c>
+      <c r="C13" s="20">
+        <v>100000</v>
+      </c>
+      <c r="D13" s="20">
+        <v>105000</v>
+      </c>
+      <c r="E13" s="20">
+        <v>180000</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10">
+        <v>3000</v>
+      </c>
+      <c r="C14" s="10">
+        <v>3000</v>
+      </c>
+      <c r="D14" s="10">
+        <v>3000</v>
+      </c>
+      <c r="E14" s="10">
+        <v>4000</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="10">
+        <f>SUM(B9:B12)</f>
+        <v>2577.5675675675675</v>
+      </c>
+      <c r="C17" s="10">
+        <f>SUM(C9:C12)</f>
+        <v>1739.9999999999975</v>
+      </c>
+      <c r="D17" s="10">
+        <f>SUM(D9:D14)</f>
+        <v>110850</v>
+      </c>
+      <c r="E17" s="10">
+        <f>SUM(E9:E12)</f>
+        <v>3032.4324324324334</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="14">
+        <f>SUM(B17:E17)</f>
+        <v>118200</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="10">
+        <f>SUMPRODUCT(B9:B12,$C$3:$C$6)</f>
+        <v>141378.37837837875</v>
+      </c>
+      <c r="C19" s="10">
+        <f>SUMPRODUCT(C9:C12,$C$3:$C$6)</f>
+        <v>99999.999999999462</v>
+      </c>
+      <c r="D19" s="10">
+        <f>SUMPRODUCT(D9:D12,$C$3:$C$6)</f>
+        <v>105000.00000000001</v>
+      </c>
+      <c r="E19" s="10">
+        <f>SUMPRODUCT(E9:E12,$C$3:$C$6)</f>
+        <v>175621.62162162166</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="28">
+        <f>SUM(B19:E19)</f>
+        <v>521999.99999999988</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="31">
+        <f>SUMPRODUCT(F9:F12,B3:B6)</f>
+        <v>719999.99999999988</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="34">
+        <f>B21*0.9</f>
+        <v>647999.99999999988</v>
+      </c>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="27" spans="1:9" s="12" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B20:E20"/>
+  </mergeCells>
+  <dataValidations xWindow="728" yWindow="451" count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Variable cells" sqref="B9:E14" xr:uid="{62243B9C-6AE9-4FE5-A047-2CBBF6710442}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D17" formula="1"/>
+    <ignoredError sqref="C19 D19:E19 B17:C17 E17" formulaRange="1"/>
+    <ignoredError sqref="B19" formula="1" formulaRange="1"/>
+  </ignoredErrors>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392F9362-3CC0-44F7-9B92-AA7C5A5C9682}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1678,72 +2537,72 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2">
         <v>1744.2342342342067</v>
@@ -1763,10 +2622,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2">
         <v>873.33333333335838</v>
@@ -1786,10 +2645,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2">
         <v>350.00000000000057</v>
@@ -1809,10 +2668,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D12" s="2">
         <v>1832.4324324324334</v>
@@ -1832,10 +2691,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -1855,10 +2714,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
@@ -1878,10 +2737,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2">
         <v>2499.9999999999995</v>
@@ -1901,10 +2760,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -1924,10 +2783,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -1947,10 +2806,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
@@ -1970,10 +2829,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -1993,10 +2852,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D20" s="2">
         <v>1200</v>
@@ -2016,10 +2875,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D21" s="2">
         <v>833.33333333336054</v>
@@ -2039,10 +2898,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2">
         <v>866.66666666663912</v>
@@ -2062,10 +2921,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -2085,10 +2944,10 @@
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D24" s="3">
         <v>0</v>
@@ -2108,57 +2967,57 @@
     </row>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="E28" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D29" s="2">
         <v>2577.5675675675675</v>
@@ -2178,10 +3037,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D30" s="2">
         <v>2577.5675675675675</v>
@@ -2201,10 +3060,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D31" s="2">
         <v>2577.5675675675675</v>
@@ -2224,10 +3083,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D32" s="2">
         <v>1739.9999999999975</v>
@@ -2247,10 +3106,10 @@
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D33" s="2">
         <v>2850</v>
@@ -2270,10 +3129,10 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D34" s="2">
         <v>3032.4324324324334</v>
@@ -2293,10 +3152,10 @@
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D35" s="2">
         <v>141378.37837837875</v>
@@ -2316,10 +3175,10 @@
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D36" s="2">
         <v>99999.999999999462</v>
@@ -2339,10 +3198,10 @@
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D37" s="2">
         <v>105000.00000000001</v>
@@ -2362,10 +3221,10 @@
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D38" s="2">
         <v>175621.62162162166</v>
@@ -2385,10 +3244,10 @@
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D39" s="2">
         <v>4589.9999999999973</v>
@@ -2408,10 +3267,10 @@
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D40" s="2">
         <v>4589.9999999999973</v>
@@ -2431,10 +3290,10 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D41" s="2">
         <v>4799.9999999999991</v>
@@ -2454,10 +3313,10 @@
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D42" s="2">
         <v>2499.9999999999995</v>
@@ -2477,10 +3336,10 @@
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D43" s="2">
         <v>1200</v>
@@ -2500,10 +3359,10 @@
     </row>
     <row r="44" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B44" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D44" s="3">
         <v>1699.9999999999995</v>
@@ -2526,11 +3385,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC694A0-2C1C-449C-964B-8A4C0FAD3276}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48:H49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2545,429 +3406,429 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>122</v>
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="33">
+        <v>123</v>
+      </c>
+      <c r="D16" s="7">
         <v>719999.99999999988</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="7">
         <v>719999.99999999988</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>123</v>
+      <c r="B20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="34">
+        <v>44</v>
+      </c>
+      <c r="D21" s="8">
         <v>1744.2342342342067</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="8">
         <v>1744.2342342342067</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="34">
+        <v>46</v>
+      </c>
+      <c r="D22" s="8">
         <v>873.33333333335838</v>
       </c>
-      <c r="E22" s="34">
+      <c r="E22" s="8">
         <v>873.33333333335838</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="34">
+        <v>48</v>
+      </c>
+      <c r="D23" s="8">
         <v>350.00000000000057</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23" s="8">
         <v>350.00000000000057</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="34">
+        <v>50</v>
+      </c>
+      <c r="D24" s="8">
         <v>1832.4324324324334</v>
       </c>
-      <c r="E24" s="34">
+      <c r="E24" s="8">
         <v>1832.4324324324334</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="34">
-        <v>0</v>
-      </c>
-      <c r="E25" s="34">
+        <v>52</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8">
         <v>0</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="34">
-        <v>0</v>
-      </c>
-      <c r="E26" s="34">
+        <v>54</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="8">
         <v>0</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="34">
+        <v>56</v>
+      </c>
+      <c r="D27" s="8">
         <v>2499.9999999999995</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="8">
         <v>2499.9999999999995</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="34">
-        <v>0</v>
-      </c>
-      <c r="E28" s="34">
+        <v>58</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+      <c r="E28" s="8">
         <v>0</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="34">
-        <v>0</v>
-      </c>
-      <c r="E29" s="34">
+        <v>60</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+      <c r="E29" s="8">
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="34">
-        <v>0</v>
-      </c>
-      <c r="E30" s="34">
+        <v>62</v>
+      </c>
+      <c r="D30" s="8">
+        <v>0</v>
+      </c>
+      <c r="E30" s="8">
         <v>0</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="34">
-        <v>0</v>
-      </c>
-      <c r="E31" s="34">
+        <v>64</v>
+      </c>
+      <c r="D31" s="8">
+        <v>0</v>
+      </c>
+      <c r="E31" s="8">
         <v>0</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="34">
+        <v>66</v>
+      </c>
+      <c r="D32" s="8">
         <v>1200</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="8">
         <v>1200</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="34">
+        <v>68</v>
+      </c>
+      <c r="D33" s="8">
         <v>833.33333333336054</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="8">
         <v>833.33333333336054</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="34">
+        <v>70</v>
+      </c>
+      <c r="D34" s="8">
         <v>866.66666666663912</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="8">
         <v>866.66666666663912</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="34">
-        <v>0</v>
-      </c>
-      <c r="E35" s="34">
+        <v>72</v>
+      </c>
+      <c r="D35" s="8">
+        <v>0</v>
+      </c>
+      <c r="E35" s="8">
         <v>0</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="33">
-        <v>0</v>
-      </c>
-      <c r="E36" s="33">
+        <v>74</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0</v>
+      </c>
+      <c r="E36" s="7">
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="F40" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="G40" s="32" t="s">
-        <v>127</v>
+      <c r="B40" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D41" s="34">
+        <v>76</v>
+      </c>
+      <c r="D41" s="8">
         <v>2577.5675675675675</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G41" s="2">
         <v>909.72972972973048</v>
@@ -2975,39 +3836,39 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="34">
+        <v>76</v>
+      </c>
+      <c r="D42" s="8">
         <v>2577.5675675675675</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G42" s="34">
+        <v>128</v>
+      </c>
+      <c r="G42" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D43" s="34">
+        <v>76</v>
+      </c>
+      <c r="D43" s="8">
         <v>2577.5675675675675</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G43" s="2">
         <v>422.43243243243251</v>
@@ -3015,19 +3876,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" s="34">
+        <v>78</v>
+      </c>
+      <c r="D44" s="8">
         <v>1739.9999999999975</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G44" s="2">
         <v>1260.0000000000025</v>
@@ -3035,19 +3896,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D45" s="34">
+        <v>80</v>
+      </c>
+      <c r="D45" s="8">
         <v>2850</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G45" s="2">
         <v>150</v>
@@ -3055,19 +3916,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D46" s="34">
+        <v>82</v>
+      </c>
+      <c r="D46" s="8">
         <v>3032.4324324324334</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G46" s="2">
         <v>967.56756756756658</v>
@@ -3075,19 +3936,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D47" s="34">
+        <v>84</v>
+      </c>
+      <c r="D47" s="8">
         <v>141378.37837837875</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G47" s="2">
         <v>28621.621621621249</v>
@@ -3095,19 +3956,19 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48" s="34">
+        <v>86</v>
+      </c>
+      <c r="D48" s="8">
         <v>99999.999999999462</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G48" s="2">
         <v>0</v>
@@ -3115,19 +3976,19 @@
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D49" s="34">
+        <v>88</v>
+      </c>
+      <c r="D49" s="8">
         <v>105000.00000000001</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G49" s="2">
         <v>0</v>
@@ -3135,19 +3996,19 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D50" s="34">
+        <v>90</v>
+      </c>
+      <c r="D50" s="8">
         <v>175621.62162162166</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G50" s="2">
         <v>4378.3783783783438</v>
@@ -3155,19 +4016,19 @@
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B51" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D51" s="34">
+        <v>92</v>
+      </c>
+      <c r="D51" s="8">
         <v>4589.9999999999973</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G51" s="2">
         <v>1020.0000000000018</v>
@@ -3175,39 +4036,39 @@
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B52" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D52" s="34">
+        <v>92</v>
+      </c>
+      <c r="D52" s="8">
         <v>4589.9999999999973</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G52" s="34">
+        <v>128</v>
+      </c>
+      <c r="G52" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" s="34">
+        <v>94</v>
+      </c>
+      <c r="D53" s="8">
         <v>4799.9999999999991</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G53" s="2">
         <v>0</v>
@@ -3215,19 +4076,19 @@
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D54" s="34">
+        <v>96</v>
+      </c>
+      <c r="D54" s="8">
         <v>2499.9999999999995</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G54" s="2">
         <v>0</v>
@@ -3235,19 +4096,19 @@
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B55" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D55" s="34">
+        <v>98</v>
+      </c>
+      <c r="D55" s="8">
         <v>1200</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G55" s="2">
         <v>0</v>
@@ -3255,19 +4116,19 @@
     </row>
     <row r="56" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B56" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D56" s="33">
+        <v>100</v>
+      </c>
+      <c r="D56" s="7">
         <v>1699.9999999999995</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G56" s="3">
         <v>0</v>
@@ -3276,4 +4137,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6441D107-8808-498B-B3B5-58CE7DF226D7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>